<commit_message>
Added Test Data and Test Scripts for Business Portal 2.5
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/Testscript-business.xlsx
+++ b/Web/coyni/resources/Testscript-business.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PaymentsAutomation\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_Web_2.5\Clone_Business_2.5_10_07_2023\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0338E343-75EC-4073-86EA-131FA957834F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B51B70-11AE-4EA4-A9D8-F67862634660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{488935C7-27F1-48B2-A245-5B3A852851D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{488935C7-27F1-48B2-A245-5B3A852851D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="103">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -66,13 +66,493 @@
   </si>
   <si>
     <t>Keywords2</t>
+  </si>
+  <si>
+    <t>Merchant Login with valid credentials</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>testdata-merchant.xlsx,login</t>
+  </si>
+  <si>
+    <t>RunOneIteration</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Merchant</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testLogin,
+-ploginHeading,
+-pmerchEmail,
+-pmerchPassword,
+-pauthyHeading,
+-pcode,
+-psecurityKey</t>
+  </si>
+  <si>
+    <t>Merchant Login View</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testLogin,
+-ploginHeading,
+-pmerchEmail,
+-pmerchPassword,
+-pauthyHeading,
+-pcode,
+-psecurityKey,
+-pattribute</t>
+  </si>
+  <si>
+    <t>Merchant Login with invalid credentials</t>
+  </si>
+  <si>
+    <t>RunRangeOfIterations</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.merchant.tests.LoginTest,
+testLoginInvalidCredentials,
+-ploginHeading,
+-pmerchEmail,
+-pmerchPassword,
+-ptoastTitle,
+-ptoastMessage,
+-perrMessage,
+-pcolour,
+-pelementName
+</t>
+  </si>
+  <si>
+    <t>Merchant Login with invalid Authy</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.merchant.tests.LoginTest,
+testLoginWithInvalidAuthy,
+-ploginHeading,
+-pmerchEmail,
+-pmerchPassword,
+-pauthyHeading,
+-pcode,
+-perrMessage,
+-pchar
+</t>
+  </si>
+  <si>
+    <t>Verify Login With Terminated User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.merchant.tests.LoginTest,
+testLoginTerminatedUser,
+-ploginHeading,
+-pmerchEmail,
+-pmerchPassword,
+-pauthyHeading,
+-ptoastMessage,
+-ptoastTitle
+</t>
+  </si>
+  <si>
+    <t>Verify Login with phonenumber</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testLoginWithPhoneNumber,
+-ploginHeading,
+-pmerchEmail,
+-pmerchPassword,
+-pphoneHeading,
+-pcode,
+-psecurityKey</t>
+  </si>
+  <si>
+    <t>Verify Login with invalid Phone OTP</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testLoginWithInvalidPhoneOTP,
+-ploginHeading,
+-pmerchEmail,
+-pmerchPassword,
+-pphoneHeading,
+-pcode,
+-perrMessage</t>
+  </si>
+  <si>
+    <t>Verify Login With ResendOTP</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testLoginWithResendOTP,
+-ploginHeading,
+-pmerchEmail,
+-pmerchPassword,
+-pphoneHeading</t>
+  </si>
+  <si>
+    <t>Forgot email with valid credentials</t>
+  </si>
+  <si>
+    <t>testdata-merchant.xlsx,forgotEmail</t>
+  </si>
+  <si>
+    <t>forgotEmail</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testForgotEmail,
+-ploginHeading,
+-pforgotHeading,
+-pfirstName,
+-plastName,
+-pphoneNumber,
+-pverificationHeading,
+-pcode</t>
+  </si>
+  <si>
+    <t>Forgot email with invalid phone number</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testForgotEmailWithInvalidPhonenumber,
+-ploginHeading,
+-pforgotHeading,
+-pphoneNumber,
+-perrMessage,
+-pcolour,
+-pelementName</t>
+  </si>
+  <si>
+    <t>Forgot email with invalid first and last name</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testForgotEmailWithInvalidFirstAndLastName,
+-ploginHeading,
+-pforgotHeading,
+-pphoneNumber,
+-pfirstName,
+-plastName,
+-perrMessage,
+-pcolour,
+-pelementName</t>
+  </si>
+  <si>
+    <t>Forgot Email With Resend Option</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testForgotEmailWithResendOption,
+-ploginHeading,
+-pforgotHeading,
+-pphoneNumber,
+-pfirstName,
+-plastName</t>
+  </si>
+  <si>
+    <t>test Forgot Password</t>
+  </si>
+  <si>
+    <t>testdata-merchant.xlsx,forgotPassword</t>
+  </si>
+  <si>
+    <t>ForgotPassword</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testForgotPassword,
+-ploginHeading,
+-pforgotHeading,
+-pmerchEmail,
+-pverificationHeading,
+-plblEmail,
+-pcode,
+-pCreatePasswordHeading,
+-penterPassword,
+-pattribute,
+-pconfirmPassword,
+-psuccessHeading,
+-ploginHeading</t>
+  </si>
+  <si>
+    <t>Test forgot password with invalid Email</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testForgotPasswordWithInvalidEmail,
+-ploginHeading,
+-pforgotHeading,
+-pmerchEmail,
+-perrMessage,
+-pcolour,
+-pelementName</t>
+  </si>
+  <si>
+    <t>Test forgot password with invalid Email Exists</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testForgotPasswordWithInvalidEmailAlreadyExistsEmail,
+-ploginHeading,
+-pforgotHeading,
+-pmerchEmail,
+-perrMessage,
+-pcolour,
+-pelementName</t>
+  </si>
+  <si>
+    <t>Test Forgot Password with invalid phone OTP</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testForgotPasswordWithInvalidPhoneOTP,
+-ploginHeading,
+-pforgotHeading,
+-pmerchEmail,
+-pverificationHeading,
+-plblEmail,
+-pcode,
+-perrMessage</t>
+  </si>
+  <si>
+    <t>test Forgot Password with invalid enter and confirm Password</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testForgotPasswordWithInvalidPasswordFiled,
+-ploginHeading,
+-pforgotHeading,
+-pmerchEmail,
+-pverificationHeading,
+-plblEmail,
+-pcode,
+-pCreatePasswordHeading,
+-penterPassword,
+-pattribute,
+-pconfirmPassword,
+-perrMessage</t>
+  </si>
+  <si>
+    <t>Verify Forgot Password With Resend Option</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.LoginTest,
+testForgotPasswordWithResendOption,
+-ploginHeading,
+-pforgotHeading,
+-pmerchEmail</t>
+  </si>
+  <si>
+    <t>Verify Top Bar</t>
+  </si>
+  <si>
+    <t>testdata-merchant.xlsx,TopMenuBar</t>
+  </si>
+  <si>
+    <t>Top bar view</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.TopBarTest,
+testTopBarDrpDwnBtns,
+-pcssProp, 
+-pvalue, 
+-pcolor,
+-pmerchantAccountsHeading,
+-ppreferencesHeading,
+-pagreementsHeading,
+-pchangePasswordHeading,
+-ptwoStepAuthenticationHeading</t>
+  </si>
+  <si>
+    <t>Verify Side Menu Bar</t>
+  </si>
+  <si>
+    <t>testdata-merchant.xlsx,SideMenuBar</t>
+  </si>
+  <si>
+    <t>Side Menu Bar</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.SideMenuBarTest,
+testSideMenuBar,
+-pcssProp, 
+-pvalue, 
+-pcolor</t>
+  </si>
+  <si>
+    <t>Verify merchant settings page side bar</t>
+  </si>
+  <si>
+    <t>testdata-merchant.xlsx,merchantSettings</t>
+  </si>
+  <si>
+    <t>merchant settings side bar</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.MerchantSettingsTest,
+testMerchantSettingsSideBar,
+-pheading</t>
+  </si>
+  <si>
+    <t>Verify User Details View</t>
+  </si>
+  <si>
+    <t>testdata-merchant.xlsx,userDetails</t>
+  </si>
+  <si>
+    <t>User Details</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.MerchantProfileTest,
+testUserDetailsView,
+-pstatus</t>
+  </si>
+  <si>
+    <t>Verify User Details Add Image</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.MerchantProfileTest,
+testUserDetailsAddImage,
+-paccountProfileHeading,
+-pcropYourImageHeading,
+-pfolderName,
+-pfileName</t>
+  </si>
+  <si>
+    <t>Verify User Details Remove Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.merchant.tests.MerchantProfileTest,
+testUserDetailsImageRemove,
+-paccountProfileHeading,
+-premoveProfileHeading
+</t>
+  </si>
+  <si>
+    <t>Verify User Details Add Image more</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.MerchantProfileTest,
+testUserDetailsAddImageMore,
+-paccountProfileHeading,
+-pcropYourImageHeading,
+-pfolderName,
+-pfileName,
+-ptoastMessage,
+-ptoastTitle</t>
+  </si>
+  <si>
+    <t>Verify Agreements</t>
+  </si>
+  <si>
+    <t>testdata-merchant.xlsx,profile</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.merchant.tests.MerchantProfileTest,
+testAgreements,
+-pheading
+</t>
+  </si>
+  <si>
+    <t>Verify Preferences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.merchant.tests.MerchantProfileTest,
+testPreferences,
+-pdefaultAccount,
+-pdefaultAccount1
+</t>
+  </si>
+  <si>
+    <t>Verify Change Password</t>
+  </si>
+  <si>
+    <t>testdata-merchant.xlsx,changePassword</t>
+  </si>
+  <si>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.merchant.tests.MerchantProfileTest,
+testChangePassword,
+-pcode,
+-pcurrentPassword,
+-pnewPassword,
+-pconfirmPassword
+</t>
+  </si>
+  <si>
+    <t>Verify Change Password SMS</t>
+  </si>
+  <si>
+    <t>Verify Change Password invalid information</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.merchant.tests.MerchantProfileTest,
+testChangePasswordInvalidCredentials,
+-pheading,
+-pcode,
+-pcurrentPassword,
+-pnewPassword,
+-pconfirmPassword,
+-perrMessage
+</t>
+  </si>
+  <si>
+    <t>Verify LogOut</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.MerchantProfileTest,
+testLogout,
+-ploginHeading</t>
+  </si>
+  <si>
+    <t>Verify Two Step Authentication</t>
+  </si>
+  <si>
+    <t>coyni.merchant.tests.MerchantProfileTest,
+testTwoStepAuthentication,
+-pcode,
+-pcode1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,8 +574,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +598,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,10 +635,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7C5355-2526-45AF-913D-A628D7592616}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +1025,7 @@
     <col min="10" max="10" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,6 +1055,1006 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="136.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" ht="167.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added export test in business portal
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/Testscript-business.xlsx
+++ b/Web/coyni/resources/Testscript-business.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_Web_2.5\Clone_Business_2.5_10_07_2023\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoyniBusiness(2.5)\Coyni(24-07-2023)\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC96950-E84E-478A-B217-3C6D97F38D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D703023-A2AB-4879-A3C9-34ED25FF6B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{488935C7-27F1-48B2-A245-5B3A852851D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{488935C7-27F1-48B2-A245-5B3A852851D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="141">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -766,6 +766,35 @@
 -pdocumentUploadHeading,
 -psignature,
 -pagreementsHeading</t>
+  </si>
+  <si>
+    <t>Verify Export Files</t>
+  </si>
+  <si>
+    <t>testdata-business.xlsx,exportFiles</t>
+  </si>
+  <si>
+    <t>ExportFile</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.ExportsTest,
+testDownloadExportFile</t>
+  </si>
+  <si>
+    <t>Verify Export Files Bulk Download</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.ExportsTest,
+testDownloadMultipleExportFiles</t>
+  </si>
+  <si>
+    <t>Verify Export Files Bulk Trash</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.ExportsTest,
+testTrashExportFile,
+-ptitle,
+-pmessage</t>
   </si>
 </sst>
 </file>
@@ -855,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -920,6 +949,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1234,27 +1270,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7C5355-2526-45AF-913D-A628D7592616}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:AC48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="E47" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="34.85546875" customWidth="1"/>
-    <col min="9" max="9" width="43.28515625" customWidth="1"/>
-    <col min="10" max="10" width="46.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.44140625" customWidth="1"/>
+    <col min="5" max="5" width="30.109375" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" customWidth="1"/>
+    <col min="8" max="8" width="34.88671875" customWidth="1"/>
+    <col min="9" max="9" width="43.33203125" customWidth="1"/>
+    <col min="10" max="10" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1286,7 +1322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>56</v>
       </c>
@@ -1318,7 +1354,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>59</v>
       </c>
@@ -1350,7 +1386,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="136.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="136.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>60</v>
       </c>
@@ -1382,7 +1418,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>61</v>
       </c>
@@ -1414,7 +1450,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="167.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="167.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1446,7 +1482,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1478,7 +1514,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1510,7 +1546,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1542,7 +1578,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1574,7 +1610,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>23</v>
       </c>
@@ -1604,7 +1640,7 @@
       </c>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>25</v>
       </c>
@@ -1634,7 +1670,7 @@
       </c>
       <c r="J12" s="14"/>
     </row>
-    <row r="13" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1664,7 +1700,7 @@
       </c>
       <c r="J13" s="14"/>
     </row>
-    <row r="14" spans="1:12" ht="210" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
@@ -1693,7 +1729,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
@@ -1722,7 +1758,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1751,7 +1787,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>33</v>
       </c>
@@ -1780,7 +1816,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1809,7 +1845,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1838,7 +1874,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>37</v>
       </c>
@@ -1870,7 +1906,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>39</v>
       </c>
@@ -1902,7 +1938,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
         <v>129</v>
       </c>
@@ -1934,7 +1970,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>68</v>
       </c>
@@ -1966,7 +2002,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
@@ -1998,7 +2034,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>43</v>
       </c>
@@ -2030,7 +2066,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>44</v>
       </c>
@@ -2062,7 +2098,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -2094,7 +2130,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>97</v>
       </c>
@@ -2126,7 +2162,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>99</v>
       </c>
@@ -2158,7 +2194,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>101</v>
       </c>
@@ -2190,7 +2226,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>103</v>
       </c>
@@ -2222,7 +2258,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -2254,7 +2290,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>107</v>
       </c>
@@ -2286,7 +2322,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -2318,7 +2354,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>111</v>
       </c>
@@ -2350,7 +2386,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>113</v>
       </c>
@@ -2382,7 +2418,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>115</v>
       </c>
@@ -2414,7 +2450,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -2446,7 +2482,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>46</v>
       </c>
@@ -2478,7 +2514,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>48</v>
       </c>
@@ -2510,7 +2546,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
         <v>49</v>
       </c>
@@ -2542,7 +2578,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>51</v>
       </c>
@@ -2574,7 +2610,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A43" s="19" t="s">
         <v>52</v>
       </c>
@@ -2606,7 +2642,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -2638,7 +2674,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -2669,6 +2705,159 @@
       <c r="J45" s="15" t="s">
         <v>84</v>
       </c>
+    </row>
+    <row r="46" spans="1:29" ht="168" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J46" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="25"/>
+      <c r="N46" s="25"/>
+      <c r="O46" s="25"/>
+      <c r="P46" s="28"/>
+      <c r="Q46" s="28"/>
+      <c r="R46" s="28"/>
+      <c r="S46" s="28"/>
+      <c r="T46" s="28"/>
+      <c r="U46" s="28"/>
+      <c r="V46" s="28"/>
+      <c r="W46" s="28"/>
+      <c r="X46" s="28"/>
+      <c r="Y46" s="28"/>
+      <c r="Z46" s="28"/>
+      <c r="AA46" s="28"/>
+      <c r="AB46" s="28"/>
+      <c r="AC46" s="28"/>
+    </row>
+    <row r="47" spans="1:29" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J47" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="K47" s="25"/>
+      <c r="L47" s="25"/>
+      <c r="M47" s="25"/>
+      <c r="N47" s="25"/>
+      <c r="O47" s="25"/>
+      <c r="P47" s="28"/>
+      <c r="Q47" s="28"/>
+      <c r="R47" s="28"/>
+      <c r="S47" s="28"/>
+      <c r="T47" s="28"/>
+      <c r="U47" s="28"/>
+      <c r="V47" s="28"/>
+      <c r="W47" s="28"/>
+      <c r="X47" s="28"/>
+      <c r="Y47" s="28"/>
+      <c r="Z47" s="28"/>
+      <c r="AA47" s="28"/>
+      <c r="AB47" s="28"/>
+      <c r="AC47" s="28"/>
+    </row>
+    <row r="48" spans="1:29" ht="175.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J48" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25"/>
+      <c r="M48" s="25"/>
+      <c r="N48" s="25"/>
+      <c r="O48" s="25"/>
+      <c r="P48" s="28"/>
+      <c r="Q48" s="28"/>
+      <c r="R48" s="28"/>
+      <c r="S48" s="28"/>
+      <c r="T48" s="28"/>
+      <c r="U48" s="28"/>
+      <c r="V48" s="28"/>
+      <c r="W48" s="28"/>
+      <c r="X48" s="28"/>
+      <c r="Y48" s="28"/>
+      <c r="Z48" s="28"/>
+      <c r="AA48" s="28"/>
+      <c r="AB48" s="28"/>
+      <c r="AC48" s="28"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J45" xr:uid="{EA7C5355-2526-45AF-913D-A628D7592616}"/>

</xml_diff>

<commit_message>
Modified test methods in business Portal
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/Testscript-business.xlsx
+++ b/Web/coyni/resources/Testscript-business.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoyniBusiness(2.5)\Coyni(24-07-2023)\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\24Business\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D703023-A2AB-4879-A3C9-34ED25FF6B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC8705D-D2C9-4E27-8D0A-08DB168CD9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{488935C7-27F1-48B2-A245-5B3A852851D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{488935C7-27F1-48B2-A245-5B3A852851D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="184">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -104,27 +104,12 @@
     <t>Verify Login With ResendOTP</t>
   </si>
   <si>
-    <t>Forgot email with valid credentials</t>
-  </si>
-  <si>
-    <t>forgotEmail</t>
-  </si>
-  <si>
-    <t>Forgot email with invalid phone number</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
-    <t>Forgot email with invalid first and last name</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
-    <t>Forgot Email With Resend Option</t>
-  </si>
-  <si>
     <t>test Forgot Password</t>
   </si>
   <si>
@@ -225,9 +210,6 @@
   </si>
   <si>
     <t>business Login with invalid Authy</t>
-  </si>
-  <si>
-    <t>testdata-business.xlsx,forgotEmail</t>
   </si>
   <si>
     <t>testdata-business.xlsx,forgotPassword</t>
@@ -643,75 +625,6 @@
 -pphoneNumber,
 -pfirstName,
 -plastName</t>
-  </si>
-  <si>
-    <t>coyni.business.tests.LoginTest,
-testForgotPassword,
--ploginHeading,
--pforgotPasswordHeading,
--pbusinessEmail,
--pverificationHeading,
--plblEmail,
--pcode,
--pCreatePasswordHeading,
--penterPassword,
--pattribute,
--pconfirmPassword,
--psuccessHeading,
--ploginHeading</t>
-  </si>
-  <si>
-    <t>coyni.business.tests.LoginTest,
-testForgotPasswordWithInvalidEmail,
--ploginHeading,
--pforgotPasswordHeading,
--pbusinessEmail,
--perrMessage,
--pcolour,
--pelementName</t>
-  </si>
-  <si>
-    <t>coyni.business.tests.LoginTest,
-testForgotPasswordWithInvalidEmailAlreadyExistsEmail,
--ploginHeading,
--pforgotPasswordHeading,
--pbusinessEmail,
--perrMessage,
--pcolour,
--pelementName</t>
-  </si>
-  <si>
-    <t>coyni.business.tests.LoginTest,
-testForgotPasswordWithInvalidPhoneOTP,
--ploginHeading,
--pforgotPasswordHeading,
--pbusinessEmail,
--pverificationHeading,
--plblEmail,
--pcode,
--perrMessage</t>
-  </si>
-  <si>
-    <t>coyni.business.tests.LoginTest,
-testForgotPasswordWithInvalidPasswordFiled,
--ploginHeading,
--pforgotPasswordHeading,
--pbusinessEmail,
--pverificationHeading,
--plblEmail,
--pcode,
--pCreatePasswordHeading,
--penterPassword,
--pattribute,
--pconfirmPassword,
--perrMessage</t>
-  </si>
-  <si>
-    <t>coyni.business.tests.LoginTest,
-testForgotPasswordWithResendOption,
--ploginHeading,
--pforgotPasswordHeading,
--pbusinessEmail</t>
   </si>
   <si>
     <t xml:space="preserve">verify Registrartion Tracker </t>
@@ -795,6 +708,301 @@
 testTrashExportFile,
 -ptitle,
 -pmessage</t>
+  </si>
+  <si>
+    <t>Retrieve email with invalid phone number</t>
+  </si>
+  <si>
+    <t>Retrieve email with valid credentials</t>
+  </si>
+  <si>
+    <t>testdata-business.xlsx,RetrieveEmail</t>
+  </si>
+  <si>
+    <t>RetrieveEmail</t>
+  </si>
+  <si>
+    <t>Retrieve email with invalid first and last name</t>
+  </si>
+  <si>
+    <t>Retrieve Email With Resend Option</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.LoginTest,
+testForgotPassword,
+-ploginHeading,
+-pforgotHeading,
+-pbusinessEmail,
+-pverificationHeading,
+-plblEmail,
+-pcode,
+-pCreatePasswordHeading,
+-penterPassword,
+-pattribute,
+-pconfirmPassword,
+-psuccessHeading,
+-ploginHeading</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.LoginTest,
+testForgotPasswordWithInvalidEmail,
+-ploginHeading,
+-pforgotHeading,
+-pbusinessEmail,
+-perrMessage,
+-pcolour,
+-pelementName</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.LoginTest,
+testForgotPasswordWithInvalidEmailAlreadyExistsEmail,
+-ploginHeading,
+-pforgotHeading,
+-pbusinessEmail,
+-perrMessage,
+-pcolour,
+-pelementName</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.LoginTest,
+testForgotPasswordWithInvalidPhoneOTP,
+-ploginHeading,
+-pforgotHeading,
+-pbusinessEmail,
+-pverificationHeading,
+-plblEmail,
+-pcode,
+-perrMessage</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.LoginTest,
+testForgotPasswordWithResendOption,
+-ploginHeading,
+-pforgotHeading,
+-pbusinessEmail</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.LoginTest,
+testForgotPasswordWithInvalidPasswordFeild,
+-ploginHeading,
+-pforgotHeading,
+-pbusinessEmail,
+-pverificationHeading,
+-plblEmail,
+-pcode,
+-pCreatePasswordHeading,
+-penterPassword,
+-pattribute,
+-pconfirmPassword,
+-perrMessage</t>
+  </si>
+  <si>
+    <t>testAccountFeeAndLimitsView</t>
+  </si>
+  <si>
+    <t>testdata-business.xlsx,AccountFee</t>
+  </si>
+  <si>
+    <t>AccountFee</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.business.tests.LoginTest,
+testLogin,
+-ploginHeading,
+-pbusinessEmail,
+-pbusinessPassword,
+-psecurityKey
+</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.BusinessSettingsTest,
+testAccountFeeAndLimitsView,
+-paccountFeeHeading,
+-pfeeHeading</t>
+  </si>
+  <si>
+    <t>testAddDebitCard</t>
+  </si>
+  <si>
+    <t>testdata-business.xlsx,PaymentMethods</t>
+  </si>
+  <si>
+    <t>PaymentMethods</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.PaymentMethodsTest,
+testAddDebitCard,
+-pnameOnCard,
+-pcardNumber,
+-pcardExpiry,
+-paddress1,
+-paddress2,
+-pcity,
+-pzipCode,
+-pstate,
+-pcountry</t>
+  </si>
+  <si>
+    <t>testEditCard</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.PaymentMethodsTest,
+testDebitCardEdit,
+-pnameOnCard,
+-pcardExpiry,
+-paddress1,
+-paddress2,
+-pcity,
+-pzipCode,
+-pstate,
+-pcountry,
+-plast4digits</t>
+  </si>
+  <si>
+    <t>testDebitDeleteCard</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.PaymentMethodsTest,
+testDebitDeleteCard,
+-plast4digits</t>
+  </si>
+  <si>
+    <t>testBusinessSettingsCardFieldValidations</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.PaymentMethodsTest,
+testDebitCardFieldValidations,
+-pnameOnCard,
+-pcardExpiry,
+-paddress1,
+-paddress2,
+-pcity,
+-pstate,</t>
+  </si>
+  <si>
+    <t>testDebitCardWithInvalidData</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.PaymentMethodsTest,
+testDebitCardWithInvalidData,
+-pnameOnCard,
+-pcardNumber,
+-pcardExpiry,
+-paddress1,
+-paddress2,
+-pcity,
+-pzipCode,
+-pstate,
+-perrMessage</t>
+  </si>
+  <si>
+    <t>testBusinessInformation</t>
+  </si>
+  <si>
+    <t>testdata-business.xlsx,SettingsbusinessInfo</t>
+  </si>
+  <si>
+    <t>Business Settings -Business information</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.BusinessSettingsTest,
+testBusinessInformation,
+-pbusinessHeading</t>
+  </si>
+  <si>
+    <t>testEditBusinessInformationCompanyEmailInvalid</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.BusinessSettingsTest,
+testEditBusinessInformationCompanyEmailInvalid,
+-pbusinessHeading,
+-perrMessage,
+-pcolor,
+-pemailAddress,
+-pelementName</t>
+  </si>
+  <si>
+    <t>testEditBusinessInformationCompanyPhoneInvalid</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.BusinessSettingsTest,
+testEditBusinessInformationCompanyPhoneInvalid,
+-pbusinessHeading,
+-perrMessage,
+-pcolor,
+-pphoneNumber,
+-pelementName</t>
+  </si>
+  <si>
+    <t>testBusinessSettingsWallets</t>
+  </si>
+  <si>
+    <t>testdata-business.xlsx,WalletSettings</t>
+  </si>
+  <si>
+    <t>Business Settings -Wallet Settings</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.BusinessSettingsTest,
+testBusinessSettingsWallets,
+-pwalletsHeading</t>
+  </si>
+  <si>
+    <t>testBusinessSettingCancelWallet</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.BusinessSettingsTest,
+testBusinessSettingCancelWallet,
+-pcancelHeading</t>
+  </si>
+  <si>
+    <t>testBusinessSettingAddNewWallet</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.BusinessSettingsTest,
+testBusinessSettingAddNewWallet,
+-pwalletHeading,
+-pwalletName</t>
+  </si>
+  <si>
+    <t>testBusinessSettingEditWallet</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.BusinessSettingsTest,
+testBusinessSettingEditWallet,
+-pwalletNewName</t>
+  </si>
+  <si>
+    <t>testDeleteBankAccount</t>
+  </si>
+  <si>
+    <t>Business Settings -Payment Methods</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.PaymentMethodsTest,
+testDeleteBankAccount,
+-premoveHeading,
+-premoveDesc,
+-premoveDescription,
+-plast4digits</t>
+  </si>
+  <si>
+    <t>testAddBankAccount</t>
+  </si>
+  <si>
+    <t>coyni.business.tests.PaymentMethodsTest,
+testAddBankAccount,
+-pexpUserName,
+-pexpPassword</t>
   </si>
 </sst>
 </file>
@@ -884,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -956,6 +1164,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1270,27 +1484,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7C5355-2526-45AF-913D-A628D7592616}">
-  <dimension ref="A1:AC48"/>
+  <dimension ref="A1:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E47" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.44140625" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
-    <col min="6" max="6" width="26.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.88671875" customWidth="1"/>
-    <col min="8" max="8" width="34.88671875" customWidth="1"/>
-    <col min="9" max="9" width="43.33203125" customWidth="1"/>
-    <col min="10" max="10" width="46.6640625" customWidth="1"/>
+    <col min="1" max="1" width="61.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="41.28515625" customWidth="1"/>
+    <col min="8" max="8" width="34.85546875" customWidth="1"/>
+    <col min="9" max="9" width="50.28515625" customWidth="1"/>
+    <col min="10" max="10" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1322,15 +1536,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -1345,24 +1559,24 @@
         <v>13</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -1377,24 +1591,24 @@
         <v>13</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="136.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="136.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
@@ -1409,24 +1623,24 @@
         <v>13</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>14</v>
@@ -1441,24 +1655,24 @@
         <v>13</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="167.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="167.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -1473,24 +1687,24 @@
         <v>13</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -1505,24 +1719,24 @@
         <v>13</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>14</v>
@@ -1537,24 +1751,24 @@
         <v>13</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
@@ -1569,24 +1783,24 @@
         <v>13</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>11</v>
@@ -1598,27 +1812,27 @@
         <v>12</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>14</v>
@@ -1627,28 +1841,28 @@
         <v>12</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>25</v>
+        <v>133</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>14</v>
@@ -1657,28 +1871,28 @@
         <v>12</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J12" s="14"/>
     </row>
-    <row r="13" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>11</v>
@@ -1690,25 +1904,25 @@
         <v>12</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J13" s="14"/>
     </row>
-    <row r="14" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="210" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>11</v>
@@ -1720,24 +1934,24 @@
         <v>12</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>14</v>
@@ -1746,85 +1960,85 @@
         <v>12</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="B18" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>14</v>
@@ -1833,312 +2047,312 @@
         <v>12</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="H21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="B24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="10" t="s">
+      <c r="H24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+      <c r="B25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="10" t="s">
+      <c r="B26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="D26" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="10" t="s">
+      <c r="B27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J27" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J26" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J27" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>14</v>
@@ -2147,30 +2361,30 @@
         <v>12</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>14</v>
@@ -2179,30 +2393,30 @@
         <v>12</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H29" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="I29" s="6" t="s">
+    </row>
+    <row r="30" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="J29" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>14</v>
@@ -2211,62 +2425,62 @@
         <v>12</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="J31" s="21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>11</v>
@@ -2278,27 +2492,27 @@
         <v>12</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>14</v>
@@ -2307,30 +2521,30 @@
         <v>12</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>11</v>
@@ -2342,27 +2556,27 @@
         <v>12</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>14</v>
@@ -2371,30 +2585,30 @@
         <v>12</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="J35" s="21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>14</v>
@@ -2403,158 +2617,158 @@
         <v>12</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G37" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" ht="135" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H37" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J37" s="17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>117</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="4" t="s">
+      <c r="H39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" ht="135" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H38" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J38" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="H40" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J40" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D41" s="20" t="s">
         <v>14</v>
@@ -2563,30 +2777,30 @@
         <v>12</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J41" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D42" s="20" t="s">
         <v>14</v>
@@ -2595,30 +2809,30 @@
         <v>12</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>14</v>
@@ -2627,62 +2841,62 @@
         <v>12</v>
       </c>
       <c r="F43" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="I43" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" ht="135" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J44" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" ht="135" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>50</v>
       </c>
-      <c r="H43" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J43" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J44" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:29" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>55</v>
-      </c>
       <c r="B45" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>11</v>
@@ -2694,27 +2908,27 @@
         <v>12</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J45" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:29" ht="168" customHeight="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>11</v>
@@ -2726,16 +2940,16 @@
         <v>12</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J46" s="27" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="K46" s="25"/>
       <c r="L46" s="25"/>
@@ -2757,15 +2971,15 @@
       <c r="AB46" s="28"/>
       <c r="AC46" s="28"/>
     </row>
-    <row r="47" spans="1:29" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D47" s="25" t="s">
         <v>11</v>
@@ -2777,16 +2991,16 @@
         <v>12</v>
       </c>
       <c r="G47" s="25" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J47" s="27" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K47" s="25"/>
       <c r="L47" s="25"/>
@@ -2808,15 +3022,15 @@
       <c r="AB47" s="28"/>
       <c r="AC47" s="28"/>
     </row>
-    <row r="48" spans="1:29" ht="175.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>11</v>
@@ -2828,16 +3042,16 @@
         <v>12</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J48" s="27" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="K48" s="25"/>
       <c r="L48" s="25"/>
@@ -2859,6 +3073,486 @@
       <c r="AB48" s="28"/>
       <c r="AC48" s="28"/>
     </row>
+    <row r="49" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J50" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A51" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J51" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A52" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A53" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J53" s="22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A54" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J54" s="22" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A55" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A56" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A57" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J58" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A59" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A60" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A61" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A62" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J62" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J63" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J45" xr:uid="{EA7C5355-2526-45AF-913D-A628D7592616}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>